<commit_message>
Scripts Catalogo y tablas
Nuevos Scripts: Catalogo y tablas
</commit_message>
<xml_diff>
--- a/IC4301_ProyectoNo1_DistribuciónTrabajo-SamanthaArburola-MarielaBarrantes.xlsx
+++ b/IC4301_ProyectoNo1_DistribuciónTrabajo-SamanthaArburola-MarielaBarrantes.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="126">
   <si>
     <t>Proyecto No 1</t>
   </si>
@@ -421,6 +421,24 @@
   </si>
   <si>
     <t>Lugar</t>
+  </si>
+  <si>
+    <t>T2-Tabla_Email</t>
+  </si>
+  <si>
+    <t>C26-Catalogo_Ciudad</t>
+  </si>
+  <si>
+    <t>C34-Catalogo_Contextura</t>
+  </si>
+  <si>
+    <t>C38-Catalogo_Cojos</t>
+  </si>
+  <si>
+    <t>C60-Catalogo_Escaolaridad</t>
+  </si>
+  <si>
+    <t>C46-Catalogo_Ocupacion</t>
   </si>
 </sst>
 </file>
@@ -896,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:I80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,9 +1014,11 @@
         <v>82</v>
       </c>
       <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+      <c r="D9" s="8" t="s">
+        <v>120</v>
+      </c>
       <c r="E9" s="8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>34</v>
@@ -1431,9 +1451,11 @@
         <v>11</v>
       </c>
       <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
+      <c r="D33" s="8" t="s">
+        <v>121</v>
+      </c>
       <c r="E33" s="8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>34</v>
@@ -1575,9 +1597,11 @@
         <v>15</v>
       </c>
       <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
+      <c r="D41" s="8" t="s">
+        <v>122</v>
+      </c>
       <c r="E41" s="8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F41" s="8" t="s">
         <v>34</v>
@@ -1647,9 +1671,11 @@
         <v>17</v>
       </c>
       <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
+      <c r="D45" s="8" t="s">
+        <v>123</v>
+      </c>
       <c r="E45" s="8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>34</v>
@@ -1791,9 +1817,11 @@
         <v>21</v>
       </c>
       <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
+      <c r="D53" s="8" t="s">
+        <v>125</v>
+      </c>
       <c r="E53" s="8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F53" s="8" t="s">
         <v>34</v>
@@ -2046,8 +2074,11 @@
       <c r="B67" t="s">
         <v>118</v>
       </c>
+      <c r="D67" t="s">
+        <v>124</v>
+      </c>
       <c r="E67" s="6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F67" t="s">
         <v>34</v>

</xml_diff>